<commit_message>
Changes of 22nd June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE Automation NegFlow.xlsx
+++ b/RTE/src/main/resources/RTE Automation NegFlow.xlsx
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" workbookViewId="0">
-      <selection activeCell="CA2" sqref="CA2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1039,7 @@
         <v>93</v>
       </c>
       <c r="P2" s="1">
-        <v>44729</v>
+        <v>44734</v>
       </c>
       <c r="Q2" s="1">
         <v>52993</v>
@@ -1048,10 +1048,10 @@
         <v>83</v>
       </c>
       <c r="S2" s="2">
-        <v>0.29166666666666669</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="T2" s="2">
-        <v>0.28125</v>
+        <v>0.90625</v>
       </c>
       <c r="U2" t="s">
         <v>84</v>
@@ -1103,10 +1103,10 @@
         <v>87</v>
       </c>
       <c r="CA2" s="1">
-        <v>44729</v>
+        <v>44734</v>
       </c>
       <c r="CB2" s="2">
-        <v>0.29166666666666669</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="CC2">
         <v>0</v>

</xml_diff>